<commit_message>
Test Extraction on Git ✨ 03 ก.พ. 64 เวลา 22:25
</commit_message>
<xml_diff>
--- a/New Wave Data🔥/xlsx/new-wave-tracker.xlsx
+++ b/New Wave Data🔥/xlsx/new-wave-tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="245">
   <si>
     <t>id</t>
   </si>
@@ -64,6 +64,9 @@
     <t>confirmed</t>
   </si>
   <si>
+    <t>unspecified_location</t>
+  </si>
+  <si>
     <t>sanitizing</t>
   </si>
   <si>
@@ -505,9 +508,18 @@
     <t>Big C เคหะร่มเกล้า</t>
   </si>
   <si>
+    <t>ตลาดบางแค</t>
+  </si>
+  <si>
+    <t>ซีคอน บางแค</t>
+  </si>
+  <si>
     <t>ตลาดนัดสายไหม</t>
   </si>
   <si>
+    <t>โรงงานแถว ถ.เพชรเกษม เขตภาษีเจริญ</t>
+  </si>
+  <si>
     <t>polli's cafe</t>
   </si>
   <si>
@@ -616,6 +628,9 @@
     <t>ไอคอนสยาม สั่งปิดร้านภายในศูนย์การค้า หลังพบพนักงานติดโควิด</t>
   </si>
   <si>
+    <t xml:space="preserve"> กทม.เปิดไทม์ไลน์ ผู้ป่วยโควิด  ประจำวันที่  3 กพ.</t>
+  </si>
+  <si>
     <t>ตลาดนัดสายไหม​แจ้งผลตรวจเชื้อโควิด-19 ของผู้ค้าในแผง​ ข้าวมันไก่ เป็นบวก 1 ราย</t>
   </si>
   <si>
@@ -722,6 +737,9 @@
   </si>
   <si>
     <t>https://today.line.me/th/v2/article/0WaWGl</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/earthpongsakornk/posts/456692252407342</t>
   </si>
   <si>
     <t>https://web.facebook.com/permalink.php?story_fbid=2793010280917181&amp;id=2007100666174817</t>
@@ -1105,7 +1123,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N153"/>
+  <dimension ref="A1:N156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1166,7 +1184,7 @@
         <v>44203</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>13.71764635</v>
@@ -1190,10 +1208,10 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -1210,7 +1228,7 @@
         <v>44203</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3">
         <v>13.7604043</v>
@@ -1234,10 +1252,10 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -1254,7 +1272,7 @@
         <v>44203</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4">
         <v>13.1501537</v>
@@ -1275,13 +1293,13 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="L4" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1298,7 +1316,7 @@
         <v>44203</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5">
         <v>13.15913922</v>
@@ -1319,13 +1337,13 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="L5" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1342,7 +1360,7 @@
         <v>44203</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6">
         <v>13.0910399</v>
@@ -1363,13 +1381,13 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="L6" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1386,7 +1404,7 @@
         <v>44203</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7">
         <v>13.16589022</v>
@@ -1410,10 +1428,10 @@
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -1430,7 +1448,7 @@
         <v>44203</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8">
         <v>13.86036949</v>
@@ -1454,10 +1472,10 @@
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -1474,7 +1492,7 @@
         <v>44203</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9">
         <v>13.8114732</v>
@@ -1498,10 +1516,10 @@
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -1518,7 +1536,7 @@
         <v>44203</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10">
         <v>13.77249026</v>
@@ -1542,10 +1560,10 @@
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -1562,7 +1580,7 @@
         <v>44203</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11">
         <v>13.81282763</v>
@@ -1586,10 +1604,10 @@
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -1606,7 +1624,7 @@
         <v>44203</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E12">
         <v>13.78500231</v>
@@ -1630,10 +1648,10 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -1650,7 +1668,7 @@
         <v>44203</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E13">
         <v>13.66376865</v>
@@ -1674,10 +1692,10 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -1694,7 +1712,7 @@
         <v>44203</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E14">
         <v>13.72626379</v>
@@ -1718,10 +1736,10 @@
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -1738,7 +1756,7 @@
         <v>44203</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E15">
         <v>13.66453742</v>
@@ -1762,10 +1780,10 @@
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -1782,7 +1800,7 @@
         <v>44203</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E16">
         <v>13.71305902</v>
@@ -1806,10 +1824,10 @@
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="N16">
         <v>0</v>
@@ -1826,7 +1844,7 @@
         <v>44203</v>
       </c>
       <c r="D17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E17">
         <v>13.74564523</v>
@@ -1850,10 +1868,10 @@
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="N17">
         <v>0</v>
@@ -1870,7 +1888,7 @@
         <v>44203</v>
       </c>
       <c r="D18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E18">
         <v>13.75690741</v>
@@ -1894,10 +1912,10 @@
         <v>0</v>
       </c>
       <c r="L18" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="N18">
         <v>0</v>
@@ -1914,7 +1932,7 @@
         <v>44203</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E19">
         <v>13.77926195</v>
@@ -1938,10 +1956,10 @@
         <v>0</v>
       </c>
       <c r="L19" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="N19">
         <v>0</v>
@@ -1958,7 +1976,7 @@
         <v>44204</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E20">
         <v>13.73456744</v>
@@ -1982,10 +2000,10 @@
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="N20">
         <v>0</v>
@@ -2002,7 +2020,7 @@
         <v>44204</v>
       </c>
       <c r="D21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E21">
         <v>13.16488063</v>
@@ -2026,10 +2044,10 @@
         <v>0</v>
       </c>
       <c r="L21" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="N21">
         <v>0</v>
@@ -2046,7 +2064,7 @@
         <v>44204</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E22">
         <v>13.84191493</v>
@@ -2070,10 +2088,10 @@
         <v>0</v>
       </c>
       <c r="L22" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="N22">
         <v>0</v>
@@ -2090,7 +2108,7 @@
         <v>44204</v>
       </c>
       <c r="D23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E23">
         <v>13.79473457</v>
@@ -2114,10 +2132,10 @@
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -2134,7 +2152,7 @@
         <v>44204</v>
       </c>
       <c r="D24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E24">
         <v>13.80561361</v>
@@ -2158,10 +2176,10 @@
         <v>0</v>
       </c>
       <c r="L24" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="N24">
         <v>0</v>
@@ -2178,7 +2196,7 @@
         <v>44204</v>
       </c>
       <c r="D25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E25">
         <v>13.45935386</v>
@@ -2202,10 +2220,10 @@
         <v>0</v>
       </c>
       <c r="L25" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -2222,7 +2240,7 @@
         <v>44204</v>
       </c>
       <c r="D26" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E26">
         <v>13.80560721</v>
@@ -2246,10 +2264,10 @@
         <v>0</v>
       </c>
       <c r="L26" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="N26">
         <v>0</v>
@@ -2266,7 +2284,7 @@
         <v>44204</v>
       </c>
       <c r="D27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E27">
         <v>13.69755718</v>
@@ -2290,10 +2308,10 @@
         <v>0</v>
       </c>
       <c r="L27" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="N27">
         <v>0</v>
@@ -2310,7 +2328,7 @@
         <v>44204</v>
       </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E28">
         <v>13.69805379</v>
@@ -2334,10 +2352,10 @@
         <v>0</v>
       </c>
       <c r="L28" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="N28">
         <v>0</v>
@@ -2354,7 +2372,7 @@
         <v>44204</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E29">
         <v>13.81037251</v>
@@ -2378,10 +2396,10 @@
         <v>0</v>
       </c>
       <c r="L29" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="N29">
         <v>0</v>
@@ -2398,7 +2416,7 @@
         <v>44205</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E30">
         <v>13.11036413</v>
@@ -2422,10 +2440,10 @@
         <v>0</v>
       </c>
       <c r="L30" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="N30">
         <v>0</v>
@@ -2442,7 +2460,7 @@
         <v>44205</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E31">
         <v>13.86194322</v>
@@ -2466,10 +2484,10 @@
         <v>0</v>
       </c>
       <c r="L31" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="N31">
         <v>0</v>
@@ -2486,7 +2504,7 @@
         <v>44205</v>
       </c>
       <c r="D32" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E32">
         <v>13.16181695</v>
@@ -2510,10 +2528,10 @@
         <v>0</v>
       </c>
       <c r="L32" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="N32">
         <v>0</v>
@@ -2530,7 +2548,7 @@
         <v>44205</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E33">
         <v>13.16787424</v>
@@ -2554,10 +2572,10 @@
         <v>0</v>
       </c>
       <c r="L33" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="N33">
         <v>0</v>
@@ -2574,7 +2592,7 @@
         <v>44205</v>
       </c>
       <c r="D34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E34">
         <v>13.76114586</v>
@@ -2598,10 +2616,10 @@
         <v>0</v>
       </c>
       <c r="L34" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="N34">
         <v>0</v>
@@ -2618,7 +2636,7 @@
         <v>44205</v>
       </c>
       <c r="D35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E35">
         <v>13.80414444</v>
@@ -2642,10 +2660,10 @@
         <v>0</v>
       </c>
       <c r="L35" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="N35">
         <v>0</v>
@@ -2662,7 +2680,7 @@
         <v>44205</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E36">
         <v>13.66420304</v>
@@ -2686,10 +2704,10 @@
         <v>0</v>
       </c>
       <c r="L36" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="N36">
         <v>0</v>
@@ -2706,7 +2724,7 @@
         <v>44205</v>
       </c>
       <c r="D37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E37">
         <v>13.66888863</v>
@@ -2730,10 +2748,10 @@
         <v>0</v>
       </c>
       <c r="L37" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="N37">
         <v>0</v>
@@ -2750,7 +2768,7 @@
         <v>44205</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E38">
         <v>13.69119413</v>
@@ -2774,10 +2792,10 @@
         <v>0</v>
       </c>
       <c r="L38" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="N38">
         <v>0</v>
@@ -2794,7 +2812,7 @@
         <v>44206</v>
       </c>
       <c r="D39" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E39">
         <v>13.71656113</v>
@@ -2818,10 +2836,10 @@
         <v>0</v>
       </c>
       <c r="L39" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="N39">
         <v>0</v>
@@ -2838,7 +2856,7 @@
         <v>44206</v>
       </c>
       <c r="D40" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E40">
         <v>13.716139</v>
@@ -2862,10 +2880,10 @@
         <v>0</v>
       </c>
       <c r="L40" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="N40">
         <v>0</v>
@@ -2882,7 +2900,7 @@
         <v>44206</v>
       </c>
       <c r="D41" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E41">
         <v>13.71882479</v>
@@ -2906,10 +2924,10 @@
         <v>0</v>
       </c>
       <c r="L41" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="N41">
         <v>0</v>
@@ -2926,7 +2944,7 @@
         <v>44206</v>
       </c>
       <c r="D42" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E42">
         <v>13.88099633</v>
@@ -2950,10 +2968,10 @@
         <v>0</v>
       </c>
       <c r="L42" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="N42">
         <v>0</v>
@@ -2970,7 +2988,7 @@
         <v>44206</v>
       </c>
       <c r="D43" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E43">
         <v>13.68095074</v>
@@ -2994,10 +3012,10 @@
         <v>0</v>
       </c>
       <c r="L43" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="N43">
         <v>0</v>
@@ -3014,7 +3032,7 @@
         <v>44206</v>
       </c>
       <c r="D44" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E44">
         <v>13.79941413</v>
@@ -3038,10 +3056,10 @@
         <v>0</v>
       </c>
       <c r="L44" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="N44">
         <v>0</v>
@@ -3058,7 +3076,7 @@
         <v>44206</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E45">
         <v>13.70244197</v>
@@ -3082,10 +3100,10 @@
         <v>0</v>
       </c>
       <c r="L45" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="N45">
         <v>0</v>
@@ -3102,7 +3120,7 @@
         <v>44206</v>
       </c>
       <c r="D46" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E46">
         <v>13.6044541</v>
@@ -3126,10 +3144,10 @@
         <v>0</v>
       </c>
       <c r="L46" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="N46">
         <v>0</v>
@@ -3146,7 +3164,7 @@
         <v>44206</v>
       </c>
       <c r="D47" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E47">
         <v>13.76023419</v>
@@ -3170,10 +3188,10 @@
         <v>0</v>
       </c>
       <c r="L47" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="N47">
         <v>0</v>
@@ -3190,7 +3208,7 @@
         <v>44206</v>
       </c>
       <c r="D48" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E48">
         <v>13.72394866</v>
@@ -3214,10 +3232,10 @@
         <v>0</v>
       </c>
       <c r="L48" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="N48">
         <v>0</v>
@@ -3234,7 +3252,7 @@
         <v>44206</v>
       </c>
       <c r="D49" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E49">
         <v>13.78259045</v>
@@ -3258,10 +3276,10 @@
         <v>0</v>
       </c>
       <c r="L49" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="N49">
         <v>0</v>
@@ -3278,7 +3296,7 @@
         <v>44206</v>
       </c>
       <c r="D50" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E50">
         <v>13.75996845</v>
@@ -3302,10 +3320,10 @@
         <v>0</v>
       </c>
       <c r="L50" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="N50">
         <v>0</v>
@@ -3322,7 +3340,7 @@
         <v>44207</v>
       </c>
       <c r="D51" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E51">
         <v>13.68517357</v>
@@ -3346,10 +3364,10 @@
         <v>0</v>
       </c>
       <c r="L51" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="N51">
         <v>0</v>
@@ -3366,7 +3384,7 @@
         <v>44207</v>
       </c>
       <c r="D52" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E52">
         <v>13.71764195</v>
@@ -3390,10 +3408,10 @@
         <v>0</v>
       </c>
       <c r="L52" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="M52" s="3" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="N52">
         <v>0</v>
@@ -3410,7 +3428,7 @@
         <v>44207</v>
       </c>
       <c r="D53" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E53">
         <v>13.96188176</v>
@@ -3434,10 +3452,10 @@
         <v>0</v>
       </c>
       <c r="L53" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="N53">
         <v>0</v>
@@ -3454,7 +3472,7 @@
         <v>44207</v>
       </c>
       <c r="D54" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E54">
         <v>13.69104063</v>
@@ -3478,10 +3496,10 @@
         <v>0</v>
       </c>
       <c r="L54" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="N54">
         <v>0</v>
@@ -3498,7 +3516,7 @@
         <v>44207</v>
       </c>
       <c r="D55" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E55">
         <v>13.8580228</v>
@@ -3522,10 +3540,10 @@
         <v>0</v>
       </c>
       <c r="L55" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="N55">
         <v>0</v>
@@ -3542,7 +3560,7 @@
         <v>44207</v>
       </c>
       <c r="D56" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E56">
         <v>13.75987349</v>
@@ -3566,10 +3584,10 @@
         <v>0</v>
       </c>
       <c r="L56" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="N56">
         <v>0</v>
@@ -3586,7 +3604,7 @@
         <v>44208</v>
       </c>
       <c r="D57" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E57">
         <v>13.87094307</v>
@@ -3610,10 +3628,10 @@
         <v>0</v>
       </c>
       <c r="L57" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="N57">
         <v>0</v>
@@ -3630,7 +3648,7 @@
         <v>44208</v>
       </c>
       <c r="D58" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E58">
         <v>13.76602425</v>
@@ -3654,10 +3672,10 @@
         <v>0</v>
       </c>
       <c r="L58" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="N58">
         <v>0</v>
@@ -3674,7 +3692,7 @@
         <v>44208</v>
       </c>
       <c r="D59" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E59">
         <v>13.76630614</v>
@@ -3698,10 +3716,10 @@
         <v>0</v>
       </c>
       <c r="L59" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="N59">
         <v>0</v>
@@ -3718,7 +3736,7 @@
         <v>44209</v>
       </c>
       <c r="D60" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E60">
         <v>13.98572175</v>
@@ -3742,10 +3760,10 @@
         <v>0</v>
       </c>
       <c r="L60" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="N60">
         <v>0</v>
@@ -3762,7 +3780,7 @@
         <v>44209</v>
       </c>
       <c r="D61" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E61">
         <v>13.98404263</v>
@@ -3786,10 +3804,10 @@
         <v>0</v>
       </c>
       <c r="L61" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="N61">
         <v>0</v>
@@ -3806,7 +3824,7 @@
         <v>44210</v>
       </c>
       <c r="D62" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E62">
         <v>13.85814935</v>
@@ -3830,10 +3848,10 @@
         <v>0</v>
       </c>
       <c r="L62" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="N62">
         <v>0</v>
@@ -3850,7 +3868,7 @@
         <v>44210</v>
       </c>
       <c r="D63" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E63">
         <v>13.66198264</v>
@@ -3874,10 +3892,10 @@
         <v>0</v>
       </c>
       <c r="L63" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="N63">
         <v>0</v>
@@ -3894,7 +3912,7 @@
         <v>44210</v>
       </c>
       <c r="D64" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E64">
         <v>13.85538476</v>
@@ -3918,10 +3936,10 @@
         <v>0</v>
       </c>
       <c r="L64" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="N64">
         <v>0</v>
@@ -3938,7 +3956,7 @@
         <v>44210</v>
       </c>
       <c r="D65" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E65">
         <v>13.79040131</v>
@@ -3962,10 +3980,10 @@
         <v>0</v>
       </c>
       <c r="L65" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="N65">
         <v>0</v>
@@ -3982,7 +4000,7 @@
         <v>44211</v>
       </c>
       <c r="D66" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E66">
         <v>13.86007893</v>
@@ -4006,10 +4024,10 @@
         <v>0</v>
       </c>
       <c r="L66" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="M66" s="3" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="N66">
         <v>0</v>
@@ -4026,7 +4044,7 @@
         <v>44211</v>
       </c>
       <c r="D67" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E67">
         <v>13.75896007</v>
@@ -4050,10 +4068,10 @@
         <v>0</v>
       </c>
       <c r="L67" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="M67" s="3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="N67">
         <v>0</v>
@@ -4070,7 +4088,7 @@
         <v>44211</v>
       </c>
       <c r="D68" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E68">
         <v>13.79943123</v>
@@ -4094,10 +4112,10 @@
         <v>0</v>
       </c>
       <c r="L68" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="M68" s="3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="N68">
         <v>0</v>
@@ -4114,7 +4132,7 @@
         <v>44211</v>
       </c>
       <c r="D69" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E69">
         <v>13.75775715</v>
@@ -4138,10 +4156,10 @@
         <v>0</v>
       </c>
       <c r="L69" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="M69" s="3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="N69">
         <v>0</v>
@@ -4158,7 +4176,7 @@
         <v>44211</v>
       </c>
       <c r="D70" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E70">
         <v>13.75776073</v>
@@ -4182,10 +4200,10 @@
         <v>0</v>
       </c>
       <c r="L70" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="M70" s="3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="N70">
         <v>0</v>
@@ -4202,7 +4220,7 @@
         <v>44211</v>
       </c>
       <c r="D71" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E71">
         <v>13.75871951</v>
@@ -4226,10 +4244,10 @@
         <v>0</v>
       </c>
       <c r="L71" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="M71" s="3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="N71">
         <v>0</v>
@@ -4246,7 +4264,7 @@
         <v>44211</v>
       </c>
       <c r="D72" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E72">
         <v>13.75843058</v>
@@ -4270,10 +4288,10 @@
         <v>0</v>
       </c>
       <c r="L72" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="M72" s="3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="N72">
         <v>0</v>
@@ -4290,7 +4308,7 @@
         <v>44211</v>
       </c>
       <c r="D73" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E73">
         <v>13.758469</v>
@@ -4314,10 +4332,10 @@
         <v>0</v>
       </c>
       <c r="L73" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="M73" s="3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="N73">
         <v>0</v>
@@ -4334,7 +4352,7 @@
         <v>44211</v>
       </c>
       <c r="D74" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E74">
         <v>13.7797938</v>
@@ -4358,10 +4376,10 @@
         <v>0</v>
       </c>
       <c r="L74" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="M74" s="3" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="N74">
         <v>0</v>
@@ -4378,7 +4396,7 @@
         <v>44211</v>
       </c>
       <c r="D75" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E75">
         <v>13.74280898</v>
@@ -4402,10 +4420,10 @@
         <v>0</v>
       </c>
       <c r="L75" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="M75" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="N75">
         <v>0</v>
@@ -4422,7 +4440,7 @@
         <v>44211</v>
       </c>
       <c r="D76" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E76">
         <v>13.67855302</v>
@@ -4446,10 +4464,10 @@
         <v>0</v>
       </c>
       <c r="L76" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="M76" s="3" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="N76">
         <v>0</v>
@@ -4466,7 +4484,7 @@
         <v>44212</v>
       </c>
       <c r="D77" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E77">
         <v>13.7126108</v>
@@ -4490,10 +4508,10 @@
         <v>0</v>
       </c>
       <c r="L77" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="M77" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="N77">
         <v>0</v>
@@ -4510,7 +4528,7 @@
         <v>44212</v>
       </c>
       <c r="D78" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E78">
         <v>13.72622518</v>
@@ -4534,10 +4552,10 @@
         <v>0</v>
       </c>
       <c r="L78" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="M78" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="N78">
         <v>0</v>
@@ -4554,7 +4572,7 @@
         <v>44212</v>
       </c>
       <c r="D79" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E79">
         <v>13.75818181</v>
@@ -4578,10 +4596,10 @@
         <v>0</v>
       </c>
       <c r="L79" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="M79" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="N79">
         <v>0</v>
@@ -4598,7 +4616,7 @@
         <v>44212</v>
       </c>
       <c r="D80" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E80">
         <v>13.736773</v>
@@ -4622,10 +4640,10 @@
         <v>0</v>
       </c>
       <c r="L80" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="M80" s="3" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="N80">
         <v>0</v>
@@ -4642,7 +4660,7 @@
         <v>44212</v>
       </c>
       <c r="D81" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E81">
         <v>13.74785996</v>
@@ -4666,10 +4684,10 @@
         <v>0</v>
       </c>
       <c r="L81" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="M81" s="3" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="N81">
         <v>0</v>
@@ -4686,7 +4704,7 @@
         <v>44212</v>
       </c>
       <c r="D82" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E82">
         <v>13.74150341</v>
@@ -4710,10 +4728,10 @@
         <v>0</v>
       </c>
       <c r="L82" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="M82" s="3" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="N82">
         <v>0</v>
@@ -4730,7 +4748,7 @@
         <v>44212</v>
       </c>
       <c r="D83" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E83">
         <v>13.75816968</v>
@@ -4754,10 +4772,10 @@
         <v>0</v>
       </c>
       <c r="L83" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="M83" s="3" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="N83">
         <v>0</v>
@@ -4774,7 +4792,7 @@
         <v>44213</v>
       </c>
       <c r="D84" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E84">
         <v>13.8442473</v>
@@ -4798,10 +4816,10 @@
         <v>0</v>
       </c>
       <c r="L84" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="M84" s="3" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="N84">
         <v>0</v>
@@ -4818,7 +4836,7 @@
         <v>44213</v>
       </c>
       <c r="D85" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E85">
         <v>13.7376095</v>
@@ -4842,10 +4860,10 @@
         <v>0</v>
       </c>
       <c r="L85" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="M85" s="3" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="N85">
         <v>0</v>
@@ -4862,7 +4880,7 @@
         <v>44213</v>
       </c>
       <c r="D86" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E86">
         <v>13.68865577</v>
@@ -4886,10 +4904,10 @@
         <v>0</v>
       </c>
       <c r="L86" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="M86" s="3" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="N86">
         <v>0</v>
@@ -4906,7 +4924,7 @@
         <v>44213</v>
       </c>
       <c r="D87" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E87">
         <v>13.74916406</v>
@@ -4930,10 +4948,10 @@
         <v>0</v>
       </c>
       <c r="L87" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="M87" s="3" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="N87">
         <v>0</v>
@@ -4950,7 +4968,7 @@
         <v>44213</v>
       </c>
       <c r="D88" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E88">
         <v>13.71136071</v>
@@ -4974,10 +4992,10 @@
         <v>0</v>
       </c>
       <c r="L88" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="M88" s="3" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="N88">
         <v>0</v>
@@ -4994,7 +5012,7 @@
         <v>44214</v>
       </c>
       <c r="D89" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E89">
         <v>13.85812537</v>
@@ -5018,10 +5036,10 @@
         <v>0</v>
       </c>
       <c r="L89" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="M89" s="3" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="N89">
         <v>0</v>
@@ -5038,7 +5056,7 @@
         <v>44214</v>
       </c>
       <c r="D90" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E90">
         <v>13.78228014</v>
@@ -5062,10 +5080,10 @@
         <v>0</v>
       </c>
       <c r="L90" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="M90" s="3" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="N90">
         <v>0</v>
@@ -5082,7 +5100,7 @@
         <v>44214</v>
       </c>
       <c r="D91" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E91">
         <v>13.85623503</v>
@@ -5106,10 +5124,10 @@
         <v>0</v>
       </c>
       <c r="L91" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="M91" s="3" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="N91">
         <v>0</v>
@@ -5126,7 +5144,7 @@
         <v>44214</v>
       </c>
       <c r="D92" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E92">
         <v>13.74686141</v>
@@ -5150,10 +5168,10 @@
         <v>0</v>
       </c>
       <c r="L92" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="M92" s="3" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="N92">
         <v>0</v>
@@ -5170,7 +5188,7 @@
         <v>44214</v>
       </c>
       <c r="D93" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E93">
         <v>13.74685295</v>
@@ -5194,10 +5212,10 @@
         <v>0</v>
       </c>
       <c r="L93" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="M93" s="3" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="N93">
         <v>0</v>
@@ -5214,7 +5232,7 @@
         <v>44214</v>
       </c>
       <c r="D94" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E94">
         <v>13.74622725</v>
@@ -5238,10 +5256,10 @@
         <v>0</v>
       </c>
       <c r="L94" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="M94" s="3" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="N94">
         <v>0</v>
@@ -5258,7 +5276,7 @@
         <v>44214</v>
       </c>
       <c r="D95" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E95">
         <v>13.69105638</v>
@@ -5282,10 +5300,10 @@
         <v>0</v>
       </c>
       <c r="L95" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="M95" s="3" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="N95">
         <v>0</v>
@@ -5302,7 +5320,7 @@
         <v>44215</v>
       </c>
       <c r="D96" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E96">
         <v>13.74344039</v>
@@ -5326,10 +5344,10 @@
         <v>0</v>
       </c>
       <c r="L96" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="M96" s="3" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="N96">
         <v>0</v>
@@ -5346,7 +5364,7 @@
         <v>44215</v>
       </c>
       <c r="D97" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E97">
         <v>13.74395671</v>
@@ -5370,10 +5388,10 @@
         <v>0</v>
       </c>
       <c r="L97" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="M97" s="3" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="N97">
         <v>0</v>
@@ -5390,7 +5408,7 @@
         <v>44215</v>
       </c>
       <c r="D98" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E98">
         <v>13.77018438</v>
@@ -5414,10 +5432,10 @@
         <v>0</v>
       </c>
       <c r="L98" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="M98" s="3" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="N98">
         <v>0</v>
@@ -5434,7 +5452,7 @@
         <v>44215</v>
       </c>
       <c r="D99" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E99">
         <v>13.68349666</v>
@@ -5458,10 +5476,10 @@
         <v>0</v>
       </c>
       <c r="L99" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="M99" s="3" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="N99">
         <v>0</v>
@@ -5478,7 +5496,7 @@
         <v>44215</v>
       </c>
       <c r="D100" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E100">
         <v>13.73137163</v>
@@ -5502,10 +5520,10 @@
         <v>0</v>
       </c>
       <c r="L100" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="M100" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="N100">
         <v>0</v>
@@ -5522,7 +5540,7 @@
         <v>44215</v>
       </c>
       <c r="D101" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E101">
         <v>13.71923763</v>
@@ -5546,10 +5564,10 @@
         <v>0</v>
       </c>
       <c r="L101" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="M101" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="N101">
         <v>0</v>
@@ -5566,7 +5584,7 @@
         <v>44215</v>
       </c>
       <c r="D102" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E102">
         <v>13.73037664</v>
@@ -5590,10 +5608,10 @@
         <v>0</v>
       </c>
       <c r="L102" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="M102" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="N102">
         <v>0</v>
@@ -5610,7 +5628,7 @@
         <v>44215</v>
       </c>
       <c r="D103" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E103">
         <v>13.85623413</v>
@@ -5634,10 +5652,10 @@
         <v>0</v>
       </c>
       <c r="L103" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="M103" s="3" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="N103">
         <v>0</v>
@@ -5654,7 +5672,7 @@
         <v>44215</v>
       </c>
       <c r="D104" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E104">
         <v>13.67368844</v>
@@ -5678,10 +5696,10 @@
         <v>0</v>
       </c>
       <c r="L104" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="M104" s="3" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="N104">
         <v>0</v>
@@ -5698,7 +5716,7 @@
         <v>44215</v>
       </c>
       <c r="D105" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E105">
         <v>13.65374287</v>
@@ -5722,10 +5740,10 @@
         <v>0</v>
       </c>
       <c r="L105" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M105" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N105">
         <v>0</v>
@@ -5742,7 +5760,7 @@
         <v>44215</v>
       </c>
       <c r="D106" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E106">
         <v>13.73765406</v>
@@ -5766,10 +5784,10 @@
         <v>0</v>
       </c>
       <c r="L106" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="M106" s="3" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="N106">
         <v>0</v>
@@ -5786,7 +5804,7 @@
         <v>44215</v>
       </c>
       <c r="D107" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E107">
         <v>13.73792402</v>
@@ -5810,10 +5828,10 @@
         <v>0</v>
       </c>
       <c r="L107" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="M107" s="3" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="N107">
         <v>0</v>
@@ -5830,7 +5848,7 @@
         <v>44216</v>
       </c>
       <c r="D108" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E108">
         <v>13.8162659</v>
@@ -5854,10 +5872,10 @@
         <v>0</v>
       </c>
       <c r="L108" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="M108" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="N108">
         <v>0</v>
@@ -5874,7 +5892,7 @@
         <v>44216</v>
       </c>
       <c r="D109" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E109">
         <v>13.74049535</v>
@@ -5898,10 +5916,10 @@
         <v>0</v>
       </c>
       <c r="L109" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="M109" s="3" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="N109">
         <v>0</v>
@@ -5918,7 +5936,7 @@
         <v>44216</v>
       </c>
       <c r="D110" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E110">
         <v>13.85569344</v>
@@ -5942,10 +5960,10 @@
         <v>0</v>
       </c>
       <c r="L110" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="M110" s="3" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="N110">
         <v>0</v>
@@ -5962,7 +5980,7 @@
         <v>44216</v>
       </c>
       <c r="D111" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E111">
         <v>13.74047635</v>
@@ -5986,10 +6004,10 @@
         <v>0</v>
       </c>
       <c r="L111" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="M111" s="3" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="N111">
         <v>0</v>
@@ -6006,7 +6024,7 @@
         <v>44216</v>
       </c>
       <c r="D112" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E112">
         <v>13.70508012</v>
@@ -6030,10 +6048,10 @@
         <v>0</v>
       </c>
       <c r="L112" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="M112" s="3" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="N112">
         <v>0</v>
@@ -6050,7 +6068,7 @@
         <v>44217</v>
       </c>
       <c r="D113" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E113">
         <v>13.75823859</v>
@@ -6074,10 +6092,10 @@
         <v>0</v>
       </c>
       <c r="L113" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="M113" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="N113">
         <v>0</v>
@@ -6094,7 +6112,7 @@
         <v>44217</v>
       </c>
       <c r="D114" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E114">
         <v>13.76561213</v>
@@ -6118,10 +6136,10 @@
         <v>0</v>
       </c>
       <c r="L114" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="M114" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="N114">
         <v>0</v>
@@ -6138,7 +6156,7 @@
         <v>44217</v>
       </c>
       <c r="D115" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E115">
         <v>13.76041719</v>
@@ -6162,10 +6180,10 @@
         <v>0</v>
       </c>
       <c r="L115" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="M115" s="3" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="N115">
         <v>0</v>
@@ -6182,7 +6200,7 @@
         <v>44217</v>
       </c>
       <c r="D116" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E116">
         <v>13.7354952</v>
@@ -6206,10 +6224,10 @@
         <v>0</v>
       </c>
       <c r="L116" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="M116" s="3" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="N116">
         <v>0</v>
@@ -6226,7 +6244,7 @@
         <v>44217</v>
       </c>
       <c r="D117" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E117">
         <v>13.73565939</v>
@@ -6250,10 +6268,10 @@
         <v>0</v>
       </c>
       <c r="L117" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="M117" s="3" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="N117">
         <v>0</v>
@@ -6270,7 +6288,7 @@
         <v>44217</v>
       </c>
       <c r="D118" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E118">
         <v>13.73550438</v>
@@ -6294,10 +6312,10 @@
         <v>0</v>
       </c>
       <c r="L118" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="M118" s="3" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="N118">
         <v>0</v>
@@ -6314,7 +6332,7 @@
         <v>44217</v>
       </c>
       <c r="D119" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E119">
         <v>13.73798989</v>
@@ -6338,10 +6356,10 @@
         <v>0</v>
       </c>
       <c r="L119" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="M119" s="3" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="N119">
         <v>0</v>
@@ -6358,7 +6376,7 @@
         <v>44217</v>
       </c>
       <c r="D120" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E120">
         <v>13.73816611</v>
@@ -6382,10 +6400,10 @@
         <v>0</v>
       </c>
       <c r="L120" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="M120" s="3" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="N120">
         <v>0</v>
@@ -6402,7 +6420,7 @@
         <v>44217</v>
       </c>
       <c r="D121" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E121">
         <v>13.72659217</v>
@@ -6426,10 +6444,10 @@
         <v>0</v>
       </c>
       <c r="L121" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="M121" s="3" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="N121">
         <v>0</v>
@@ -6446,7 +6464,7 @@
         <v>44217</v>
       </c>
       <c r="D122" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E122">
         <v>12.94549134</v>
@@ -6470,10 +6488,10 @@
         <v>0</v>
       </c>
       <c r="L122" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M122" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N122">
         <v>0</v>
@@ -6490,7 +6508,7 @@
         <v>44217</v>
       </c>
       <c r="D123" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E123">
         <v>13.69101533</v>
@@ -6514,10 +6532,10 @@
         <v>0</v>
       </c>
       <c r="L123" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M123" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N123">
         <v>0</v>
@@ -6534,7 +6552,7 @@
         <v>44217</v>
       </c>
       <c r="D124" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E124">
         <v>13.71007281</v>
@@ -6558,10 +6576,10 @@
         <v>0</v>
       </c>
       <c r="L124" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="M124" s="3" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="N124">
         <v>0</v>
@@ -6578,7 +6596,7 @@
         <v>44218</v>
       </c>
       <c r="D125" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E125">
         <v>13.82881268</v>
@@ -6602,10 +6620,10 @@
         <v>0</v>
       </c>
       <c r="L125" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="M125" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="N125">
         <v>0</v>
@@ -6622,7 +6640,7 @@
         <v>44218</v>
       </c>
       <c r="D126" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E126">
         <v>13.81119997</v>
@@ -6646,10 +6664,10 @@
         <v>0</v>
       </c>
       <c r="L126" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="M126" s="3" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="N126">
         <v>0</v>
@@ -6666,7 +6684,7 @@
         <v>44218</v>
       </c>
       <c r="D127" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E127">
         <v>13.72039971</v>
@@ -6690,10 +6708,10 @@
         <v>0</v>
       </c>
       <c r="L127" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="M127" s="3" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="N127">
         <v>0</v>
@@ -6710,7 +6728,7 @@
         <v>44218</v>
       </c>
       <c r="D128" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E128">
         <v>13.8622826</v>
@@ -6734,10 +6752,10 @@
         <v>0</v>
       </c>
       <c r="L128" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M128" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N128">
         <v>0</v>
@@ -6754,7 +6772,7 @@
         <v>44218</v>
       </c>
       <c r="D129" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E129">
         <v>13.816256</v>
@@ -6778,10 +6796,10 @@
         <v>0</v>
       </c>
       <c r="L129" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M129" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N129">
         <v>0</v>
@@ -6798,7 +6816,7 @@
         <v>44218</v>
       </c>
       <c r="D130" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E130">
         <v>0</v>
@@ -6822,10 +6840,10 @@
         <v>0</v>
       </c>
       <c r="L130" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M130" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N130">
         <v>0</v>
@@ -6842,7 +6860,7 @@
         <v>44218</v>
       </c>
       <c r="D131" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E131">
         <v>13.71297441</v>
@@ -6866,10 +6884,10 @@
         <v>0</v>
       </c>
       <c r="L131" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M131" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N131">
         <v>0</v>
@@ -6886,7 +6904,7 @@
         <v>44218</v>
       </c>
       <c r="D132" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E132">
         <v>13.72520981</v>
@@ -6910,10 +6928,10 @@
         <v>0</v>
       </c>
       <c r="L132" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M132" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N132">
         <v>0</v>
@@ -6930,7 +6948,7 @@
         <v>44218</v>
       </c>
       <c r="D133" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E133">
         <v>0</v>
@@ -6954,10 +6972,10 @@
         <v>0</v>
       </c>
       <c r="L133" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M133" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N133">
         <v>0</v>
@@ -6974,7 +6992,7 @@
         <v>44218</v>
       </c>
       <c r="D134" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E134">
         <v>13.86206011</v>
@@ -6998,10 +7016,10 @@
         <v>0</v>
       </c>
       <c r="L134" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M134" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N134">
         <v>0</v>
@@ -7018,7 +7036,7 @@
         <v>44219</v>
       </c>
       <c r="D135" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E135">
         <v>13.72659978</v>
@@ -7042,10 +7060,10 @@
         <v>0</v>
       </c>
       <c r="L135" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="M135" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="N135">
         <v>0</v>
@@ -7062,7 +7080,7 @@
         <v>44219</v>
       </c>
       <c r="D136" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E136">
         <v>13.72689292</v>
@@ -7086,10 +7104,10 @@
         <v>0</v>
       </c>
       <c r="L136" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="M136" s="3" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="N136">
         <v>0</v>
@@ -7106,7 +7124,7 @@
         <v>44219</v>
       </c>
       <c r="D137" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E137">
         <v>13.69402065</v>
@@ -7130,10 +7148,10 @@
         <v>0</v>
       </c>
       <c r="L137" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M137" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N137">
         <v>0</v>
@@ -7150,7 +7168,7 @@
         <v>44219</v>
       </c>
       <c r="D138" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E138">
         <v>13.87076529</v>
@@ -7174,10 +7192,10 @@
         <v>0</v>
       </c>
       <c r="L138" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M138" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N138">
         <v>0</v>
@@ -7194,7 +7212,7 @@
         <v>44219</v>
       </c>
       <c r="D139" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E139">
         <v>13.6800885</v>
@@ -7218,10 +7236,10 @@
         <v>0</v>
       </c>
       <c r="L139" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M139" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N139">
         <v>0</v>
@@ -7238,7 +7256,7 @@
         <v>44219</v>
       </c>
       <c r="D140" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E140">
         <v>13.65422663</v>
@@ -7262,10 +7280,10 @@
         <v>0</v>
       </c>
       <c r="L140" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M140" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N140">
         <v>0</v>
@@ -7282,7 +7300,7 @@
         <v>44219</v>
       </c>
       <c r="D141" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E141">
         <v>13.74687259</v>
@@ -7306,10 +7324,10 @@
         <v>0</v>
       </c>
       <c r="L141" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M141" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N141">
         <v>0</v>
@@ -7326,7 +7344,7 @@
         <v>44219</v>
       </c>
       <c r="D142" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E142">
         <v>13.72326345</v>
@@ -7350,10 +7368,10 @@
         <v>0</v>
       </c>
       <c r="L142" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M142" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N142">
         <v>0</v>
@@ -7370,7 +7388,7 @@
         <v>44219</v>
       </c>
       <c r="D143" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E143">
         <v>13.69129891</v>
@@ -7394,10 +7412,10 @@
         <v>0</v>
       </c>
       <c r="L143" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M143" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N143">
         <v>0</v>
@@ -7414,7 +7432,7 @@
         <v>44219</v>
       </c>
       <c r="D144" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E144">
         <v>13.68900827</v>
@@ -7438,10 +7456,10 @@
         <v>0</v>
       </c>
       <c r="L144" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M144" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N144">
         <v>0</v>
@@ -7458,7 +7476,7 @@
         <v>44219</v>
       </c>
       <c r="D145" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E145">
         <v>13.69840074</v>
@@ -7482,10 +7500,10 @@
         <v>0</v>
       </c>
       <c r="L145" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M145" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N145">
         <v>0</v>
@@ -7502,7 +7520,7 @@
         <v>44219</v>
       </c>
       <c r="D146" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E146">
         <v>13.69811266</v>
@@ -7526,10 +7544,10 @@
         <v>0</v>
       </c>
       <c r="L146" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M146" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N146">
         <v>0</v>
@@ -7546,7 +7564,7 @@
         <v>44220</v>
       </c>
       <c r="D147" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E147">
         <v>13.86747225</v>
@@ -7570,10 +7588,10 @@
         <v>0</v>
       </c>
       <c r="L147" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M147" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N147">
         <v>0</v>
@@ -7590,7 +7608,7 @@
         <v>44220</v>
       </c>
       <c r="D148" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E148">
         <v>13.82613606</v>
@@ -7614,10 +7632,10 @@
         <v>0</v>
       </c>
       <c r="L148" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M148" s="3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="N148">
         <v>0</v>
@@ -7634,7 +7652,7 @@
         <v>44220</v>
       </c>
       <c r="D149" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E149">
         <v>13.76535838</v>
@@ -7658,10 +7676,10 @@
         <v>0</v>
       </c>
       <c r="L149" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="M149" s="3" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="N149">
         <v>0</v>
@@ -7678,7 +7696,7 @@
         <v>44220</v>
       </c>
       <c r="D150" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E150">
         <v>13.86748347</v>
@@ -7702,10 +7720,10 @@
         <v>0</v>
       </c>
       <c r="L150" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="M150" s="3" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="N150">
         <v>0</v>
@@ -7719,16 +7737,16 @@
         <v>14</v>
       </c>
       <c r="C151" s="2">
-        <v>44224</v>
+        <v>44220</v>
       </c>
       <c r="D151" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E151">
-        <v>13.92160509</v>
+        <v>13.71189925</v>
       </c>
       <c r="F151">
-        <v>100.6679682</v>
+        <v>100.4275498</v>
       </c>
       <c r="G151">
         <v>0</v>
@@ -7746,10 +7764,10 @@
         <v>0</v>
       </c>
       <c r="L151" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="M151" s="3" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="N151">
         <v>0</v>
@@ -7760,19 +7778,19 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C152" s="2">
-        <v>44227</v>
+        <v>44220</v>
       </c>
       <c r="D152" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E152">
-        <v>13.72654449</v>
+        <v>13.71171772</v>
       </c>
       <c r="F152">
-        <v>100.5997291</v>
+        <v>100.4340445</v>
       </c>
       <c r="G152">
         <v>0</v>
@@ -7790,10 +7808,10 @@
         <v>0</v>
       </c>
       <c r="L152" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="M152" s="3" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="N152">
         <v>0</v>
@@ -7807,39 +7825,171 @@
         <v>14</v>
       </c>
       <c r="C153" s="2">
+        <v>44224</v>
+      </c>
+      <c r="D153" t="s">
+        <v>166</v>
+      </c>
+      <c r="E153">
+        <v>13.92160509</v>
+      </c>
+      <c r="F153">
+        <v>100.6679682</v>
+      </c>
+      <c r="G153">
+        <v>0</v>
+      </c>
+      <c r="H153">
+        <v>0</v>
+      </c>
+      <c r="I153">
+        <v>0</v>
+      </c>
+      <c r="J153">
+        <v>0</v>
+      </c>
+      <c r="K153">
+        <v>0</v>
+      </c>
+      <c r="L153" t="s">
+        <v>205</v>
+      </c>
+      <c r="M153" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="N153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14">
+      <c r="A154">
+        <v>152</v>
+      </c>
+      <c r="B154" t="s">
+        <v>16</v>
+      </c>
+      <c r="C154" s="2">
+        <v>44224</v>
+      </c>
+      <c r="D154" t="s">
+        <v>167</v>
+      </c>
+      <c r="E154">
+        <v>13.71657541</v>
+      </c>
+      <c r="F154">
+        <v>100.4430568</v>
+      </c>
+      <c r="G154">
+        <v>0</v>
+      </c>
+      <c r="H154">
+        <v>0</v>
+      </c>
+      <c r="I154">
+        <v>0</v>
+      </c>
+      <c r="J154">
+        <v>0</v>
+      </c>
+      <c r="K154">
+        <v>0</v>
+      </c>
+      <c r="L154" t="s">
+        <v>204</v>
+      </c>
+      <c r="M154" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="N154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14">
+      <c r="A155">
+        <v>153</v>
+      </c>
+      <c r="B155" t="s">
+        <v>17</v>
+      </c>
+      <c r="C155" s="2">
+        <v>44227</v>
+      </c>
+      <c r="D155" t="s">
+        <v>168</v>
+      </c>
+      <c r="E155">
+        <v>13.72654449</v>
+      </c>
+      <c r="F155">
+        <v>100.5997291</v>
+      </c>
+      <c r="G155">
+        <v>0</v>
+      </c>
+      <c r="H155">
+        <v>0</v>
+      </c>
+      <c r="I155">
+        <v>0</v>
+      </c>
+      <c r="J155">
+        <v>0</v>
+      </c>
+      <c r="K155">
+        <v>0</v>
+      </c>
+      <c r="L155" t="s">
+        <v>206</v>
+      </c>
+      <c r="M155" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="N155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14">
+      <c r="A156">
+        <v>154</v>
+      </c>
+      <c r="B156" t="s">
+        <v>14</v>
+      </c>
+      <c r="C156" s="2">
         <v>44229</v>
       </c>
-      <c r="D153" t="s">
-        <v>165</v>
-      </c>
-      <c r="E153">
+      <c r="D156" t="s">
+        <v>169</v>
+      </c>
+      <c r="E156">
         <v>14.02205306</v>
       </c>
-      <c r="F153">
+      <c r="F156">
         <v>99.99050403</v>
       </c>
-      <c r="G153">
-        <v>0</v>
-      </c>
-      <c r="H153">
-        <v>0</v>
-      </c>
-      <c r="I153">
-        <v>0</v>
-      </c>
-      <c r="J153">
-        <v>0</v>
-      </c>
-      <c r="K153">
-        <v>0</v>
-      </c>
-      <c r="L153" t="s">
-        <v>202</v>
-      </c>
-      <c r="M153" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="N153">
+      <c r="G156">
+        <v>0</v>
+      </c>
+      <c r="H156">
+        <v>0</v>
+      </c>
+      <c r="I156">
+        <v>0</v>
+      </c>
+      <c r="J156">
+        <v>0</v>
+      </c>
+      <c r="K156">
+        <v>0</v>
+      </c>
+      <c r="L156" t="s">
+        <v>207</v>
+      </c>
+      <c r="M156" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="N156">
         <v>0</v>
       </c>
     </row>
@@ -7997,6 +8147,9 @@
     <hyperlink ref="M151" r:id="rId150"/>
     <hyperlink ref="M152" r:id="rId151"/>
     <hyperlink ref="M153" r:id="rId152"/>
+    <hyperlink ref="M154" r:id="rId153"/>
+    <hyperlink ref="M155" r:id="rId154"/>
+    <hyperlink ref="M156" r:id="rId155"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Test Extraction on Git ✨ 20 ก.พ. 64 เวลา 01:13
</commit_message>
<xml_diff>
--- a/New Wave Data🔥/xlsx/new-wave-tracker.xlsx
+++ b/New Wave Data🔥/xlsx/new-wave-tracker.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="148">
   <si>
     <t>id</t>
   </si>
@@ -211,6 +211,9 @@
     <t>ป้ายรถ pop คณะเศรษฐศาสตร์ จุฬา</t>
   </si>
   <si>
+    <t>สถานฑูตเกาหลี</t>
+  </si>
+  <si>
     <t>อาคารจามจุรี 5</t>
   </si>
   <si>
@@ -241,6 +244,9 @@
     <t>BTS สถานีสยาม</t>
   </si>
   <si>
+    <t>Home Fresh Mart เดอะมอลล์ท่าพระ</t>
+  </si>
+  <si>
     <t>จุฬา ฝั่งตะวันตก</t>
   </si>
   <si>
@@ -349,6 +355,9 @@
     <t>ตลาดสี่มุมเมือง</t>
   </si>
   <si>
+    <t>ตลาดท่าดินแดง คลองสาน</t>
+  </si>
+  <si>
     <t>ไอคอนสยาม สั่งปิดร้านภายในศูนย์การค้า หลังพบพนักงานติดโควิด</t>
   </si>
   <si>
@@ -394,6 +403,9 @@
     <t>นิสิตม.เกษตร ติด 'โควิด' เผยเดินทางมาจากสมุทรสาคร หลังเปิดเรียนวันแรก</t>
   </si>
   <si>
+    <t xml:space="preserve"> กทม.เปิดไทม์ไลน์ ผู้ป่วยโควิด  ประจำวันที่  19 กพ.</t>
+  </si>
+  <si>
     <t xml:space="preserve"> กทม.เปิดไทม์ไลน์ ผู้ป่วยโควิด  ประจำวันที่  13 กพ.</t>
   </si>
   <si>
@@ -440,6 +452,9 @@
   </si>
   <si>
     <t>https://today.line.me/th/v2/article/k1kpqJ</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/earthpongsakornk/posts/466640598079174</t>
   </si>
   <si>
     <t>https://www.facebook.com/earthpongsakornk/posts/462881311788436</t>
@@ -817,7 +832,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N100"/>
+  <dimension ref="A1:N103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -902,10 +917,10 @@
         <v>0</v>
       </c>
       <c r="L2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -946,10 +961,10 @@
         <v>0</v>
       </c>
       <c r="L3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -990,10 +1005,10 @@
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1034,10 +1049,10 @@
         <v>0</v>
       </c>
       <c r="L5" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1078,10 +1093,10 @@
         <v>0</v>
       </c>
       <c r="L6" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1122,10 +1137,10 @@
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -1166,10 +1181,10 @@
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -1210,10 +1225,10 @@
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -1254,10 +1269,10 @@
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -1298,10 +1313,10 @@
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -1342,10 +1357,10 @@
         <v>0</v>
       </c>
       <c r="L12" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -1386,10 +1401,10 @@
         <v>0</v>
       </c>
       <c r="L13" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -1430,10 +1445,10 @@
         <v>0</v>
       </c>
       <c r="L14" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -1474,10 +1489,10 @@
         <v>0</v>
       </c>
       <c r="L15" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -1518,10 +1533,10 @@
         <v>0</v>
       </c>
       <c r="L16" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="N16">
         <v>0</v>
@@ -1562,10 +1577,10 @@
         <v>0</v>
       </c>
       <c r="L17" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="N17">
         <v>0</v>
@@ -1606,10 +1621,10 @@
         <v>0</v>
       </c>
       <c r="L18" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="N18">
         <v>0</v>
@@ -1650,10 +1665,10 @@
         <v>0</v>
       </c>
       <c r="L19" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="N19">
         <v>0</v>
@@ -1694,10 +1709,10 @@
         <v>0</v>
       </c>
       <c r="L20" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="N20">
         <v>0</v>
@@ -1738,10 +1753,10 @@
         <v>0</v>
       </c>
       <c r="L21" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="N21">
         <v>0</v>
@@ -1782,10 +1797,10 @@
         <v>0</v>
       </c>
       <c r="L22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="N22">
         <v>0</v>
@@ -1826,10 +1841,10 @@
         <v>0</v>
       </c>
       <c r="L23" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -1870,10 +1885,10 @@
         <v>0</v>
       </c>
       <c r="L24" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="N24">
         <v>0</v>
@@ -1914,10 +1929,10 @@
         <v>0</v>
       </c>
       <c r="L25" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -1958,10 +1973,10 @@
         <v>0</v>
       </c>
       <c r="L26" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="N26">
         <v>0</v>
@@ -2002,10 +2017,10 @@
         <v>0</v>
       </c>
       <c r="L27" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="N27">
         <v>0</v>
@@ -2046,10 +2061,10 @@
         <v>0</v>
       </c>
       <c r="L28" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="N28">
         <v>0</v>
@@ -2090,10 +2105,10 @@
         <v>0</v>
       </c>
       <c r="L29" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="N29">
         <v>0</v>
@@ -2134,10 +2149,10 @@
         <v>0</v>
       </c>
       <c r="L30" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="N30">
         <v>0</v>
@@ -2178,10 +2193,10 @@
         <v>0</v>
       </c>
       <c r="L31" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="N31">
         <v>0</v>
@@ -2222,10 +2237,10 @@
         <v>0</v>
       </c>
       <c r="L32" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="N32">
         <v>0</v>
@@ -2266,10 +2281,10 @@
         <v>0</v>
       </c>
       <c r="L33" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="N33">
         <v>0</v>
@@ -2310,10 +2325,10 @@
         <v>0</v>
       </c>
       <c r="L34" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="N34">
         <v>0</v>
@@ -2354,10 +2369,10 @@
         <v>0</v>
       </c>
       <c r="L35" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="N35">
         <v>0</v>
@@ -2398,10 +2413,10 @@
         <v>0</v>
       </c>
       <c r="L36" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="N36">
         <v>0</v>
@@ -2442,10 +2457,10 @@
         <v>0</v>
       </c>
       <c r="L37" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="N37">
         <v>0</v>
@@ -2486,10 +2501,10 @@
         <v>0</v>
       </c>
       <c r="L38" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="N38">
         <v>0</v>
@@ -2530,10 +2545,10 @@
         <v>0</v>
       </c>
       <c r="L39" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="N39">
         <v>0</v>
@@ -2574,10 +2589,10 @@
         <v>0</v>
       </c>
       <c r="L40" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="N40">
         <v>0</v>
@@ -2618,10 +2633,10 @@
         <v>0</v>
       </c>
       <c r="L41" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="N41">
         <v>0</v>
@@ -2662,10 +2677,10 @@
         <v>0</v>
       </c>
       <c r="L42" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="N42">
         <v>0</v>
@@ -2706,10 +2721,10 @@
         <v>0</v>
       </c>
       <c r="L43" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="N43">
         <v>0</v>
@@ -2750,10 +2765,10 @@
         <v>0</v>
       </c>
       <c r="L44" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="N44">
         <v>0</v>
@@ -2794,10 +2809,10 @@
         <v>0</v>
       </c>
       <c r="L45" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N45">
         <v>0</v>
@@ -2838,10 +2853,10 @@
         <v>0</v>
       </c>
       <c r="L46" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N46">
         <v>0</v>
@@ -2882,10 +2897,10 @@
         <v>0</v>
       </c>
       <c r="L47" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N47">
         <v>0</v>
@@ -2926,10 +2941,10 @@
         <v>0</v>
       </c>
       <c r="L48" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="N48">
         <v>0</v>
@@ -2970,10 +2985,10 @@
         <v>0</v>
       </c>
       <c r="L49" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="N49">
         <v>0</v>
@@ -3014,10 +3029,10 @@
         <v>0</v>
       </c>
       <c r="L50" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="N50">
         <v>0</v>
@@ -3058,10 +3073,10 @@
         <v>0</v>
       </c>
       <c r="L51" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N51">
         <v>0</v>
@@ -3075,16 +3090,16 @@
         <v>15</v>
       </c>
       <c r="C52" s="2">
-        <v>44230</v>
+        <v>44229</v>
       </c>
       <c r="D52" t="s">
         <v>65</v>
       </c>
       <c r="E52">
-        <v>13.73818758</v>
+        <v>13.76751158</v>
       </c>
       <c r="F52">
-        <v>100.5288896</v>
+        <v>100.5779559</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -3102,10 +3117,10 @@
         <v>0</v>
       </c>
       <c r="L52" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="M52" s="3" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="N52">
         <v>0</v>
@@ -3125,10 +3140,10 @@
         <v>66</v>
       </c>
       <c r="E53">
-        <v>13.65053065</v>
+        <v>13.73818758</v>
       </c>
       <c r="F53">
-        <v>100.3873459</v>
+        <v>100.5288896</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -3149,7 +3164,7 @@
         <v>121</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="N53">
         <v>0</v>
@@ -3163,16 +3178,16 @@
         <v>15</v>
       </c>
       <c r="C54" s="2">
-        <v>44231</v>
+        <v>44230</v>
       </c>
       <c r="D54" t="s">
         <v>67</v>
       </c>
       <c r="E54">
-        <v>13.74289669</v>
+        <v>13.65053065</v>
       </c>
       <c r="F54">
-        <v>100.5245605</v>
+        <v>100.3873459</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -3190,10 +3205,10 @@
         <v>0</v>
       </c>
       <c r="L54" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="N54">
         <v>0</v>
@@ -3213,10 +3228,10 @@
         <v>68</v>
       </c>
       <c r="E55">
-        <v>13.73937658</v>
+        <v>13.74289669</v>
       </c>
       <c r="F55">
-        <v>100.5293983</v>
+        <v>100.5245605</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -3234,10 +3249,10 @@
         <v>0</v>
       </c>
       <c r="L55" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="N55">
         <v>0</v>
@@ -3257,10 +3272,10 @@
         <v>69</v>
       </c>
       <c r="E56">
-        <v>13.74256403</v>
+        <v>13.73937658</v>
       </c>
       <c r="F56">
-        <v>100.5328305</v>
+        <v>100.5293983</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -3278,10 +3293,10 @@
         <v>0</v>
       </c>
       <c r="L56" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="N56">
         <v>0</v>
@@ -3301,10 +3316,10 @@
         <v>70</v>
       </c>
       <c r="E57">
-        <v>13.70822271</v>
+        <v>13.74256403</v>
       </c>
       <c r="F57">
-        <v>100.5310484</v>
+        <v>100.5328305</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -3322,10 +3337,10 @@
         <v>0</v>
       </c>
       <c r="L57" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N57">
         <v>0</v>
@@ -3345,10 +3360,10 @@
         <v>71</v>
       </c>
       <c r="E58">
-        <v>13.60021773</v>
+        <v>13.70822271</v>
       </c>
       <c r="F58">
-        <v>100.4056859</v>
+        <v>100.5310484</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -3369,7 +3384,7 @@
         <v>126</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N58">
         <v>0</v>
@@ -3389,10 +3404,10 @@
         <v>72</v>
       </c>
       <c r="E59">
-        <v>13.71174865</v>
+        <v>13.60021773</v>
       </c>
       <c r="F59">
-        <v>100.4341559</v>
+        <v>100.4056859</v>
       </c>
       <c r="G59">
         <v>0</v>
@@ -3410,10 +3425,10 @@
         <v>0</v>
       </c>
       <c r="L59" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="N59">
         <v>0</v>
@@ -3433,10 +3448,10 @@
         <v>73</v>
       </c>
       <c r="E60">
-        <v>13.736633</v>
+        <v>13.71174865</v>
       </c>
       <c r="F60">
-        <v>100.5288218</v>
+        <v>100.4341559</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -3454,10 +3469,10 @@
         <v>0</v>
       </c>
       <c r="L60" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="N60">
         <v>0</v>
@@ -3477,10 +3492,10 @@
         <v>74</v>
       </c>
       <c r="E61">
-        <v>13.74560482</v>
+        <v>13.736633</v>
       </c>
       <c r="F61">
-        <v>100.5341794</v>
+        <v>100.5288218</v>
       </c>
       <c r="G61">
         <v>0</v>
@@ -3498,10 +3513,10 @@
         <v>0</v>
       </c>
       <c r="L61" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="N61">
         <v>0</v>
@@ -3515,16 +3530,16 @@
         <v>15</v>
       </c>
       <c r="C62" s="2">
-        <v>44232</v>
+        <v>44231</v>
       </c>
       <c r="D62" t="s">
         <v>75</v>
       </c>
       <c r="E62">
-        <v>13.73982463</v>
+        <v>13.74560482</v>
       </c>
       <c r="F62">
-        <v>100.527923</v>
+        <v>100.5341794</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -3542,10 +3557,10 @@
         <v>0</v>
       </c>
       <c r="L62" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="N62">
         <v>0</v>
@@ -3559,16 +3574,16 @@
         <v>15</v>
       </c>
       <c r="C63" s="2">
-        <v>44232</v>
+        <v>44231</v>
       </c>
       <c r="D63" t="s">
         <v>76</v>
       </c>
       <c r="E63">
-        <v>13.74247791</v>
+        <v>13.71355565</v>
       </c>
       <c r="F63">
-        <v>100.5274041</v>
+        <v>100.4792722</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -3586,10 +3601,10 @@
         <v>0</v>
       </c>
       <c r="L63" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="N63">
         <v>0</v>
@@ -3609,10 +3624,10 @@
         <v>77</v>
       </c>
       <c r="E64">
-        <v>13.74488629</v>
+        <v>13.73982463</v>
       </c>
       <c r="F64">
-        <v>100.5316173</v>
+        <v>100.527923</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -3630,10 +3645,10 @@
         <v>0</v>
       </c>
       <c r="L64" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="N64">
         <v>0</v>
@@ -3653,10 +3668,10 @@
         <v>78</v>
       </c>
       <c r="E65">
-        <v>13.74090896</v>
+        <v>13.74247791</v>
       </c>
       <c r="F65">
-        <v>100.5283409</v>
+        <v>100.5274041</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -3674,10 +3689,10 @@
         <v>0</v>
       </c>
       <c r="L65" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N65">
         <v>0</v>
@@ -3697,10 +3712,10 @@
         <v>79</v>
       </c>
       <c r="E66">
-        <v>13.74064196</v>
+        <v>13.74488629</v>
       </c>
       <c r="F66">
-        <v>100.5270177</v>
+        <v>100.5316173</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -3718,10 +3733,10 @@
         <v>0</v>
       </c>
       <c r="L66" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M66" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N66">
         <v>0</v>
@@ -3741,10 +3756,10 @@
         <v>80</v>
       </c>
       <c r="E67">
-        <v>13.74172094</v>
+        <v>13.74090896</v>
       </c>
       <c r="F67">
-        <v>100.5260114</v>
+        <v>100.5283409</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -3762,10 +3777,10 @@
         <v>0</v>
       </c>
       <c r="L67" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="M67" s="3" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="N67">
         <v>0</v>
@@ -3785,10 +3800,10 @@
         <v>81</v>
       </c>
       <c r="E68">
-        <v>13.74157164</v>
+        <v>13.74064196</v>
       </c>
       <c r="F68">
-        <v>100.5295636</v>
+        <v>100.5270177</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -3806,10 +3821,10 @@
         <v>0</v>
       </c>
       <c r="L68" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="M68" s="3" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="N68">
         <v>0</v>
@@ -3829,10 +3844,10 @@
         <v>82</v>
       </c>
       <c r="E69">
-        <v>13.73967506</v>
+        <v>13.74172094</v>
       </c>
       <c r="F69">
-        <v>100.5262292</v>
+        <v>100.5260114</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -3850,10 +3865,10 @@
         <v>0</v>
       </c>
       <c r="L69" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="M69" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="N69">
         <v>0</v>
@@ -3873,10 +3888,10 @@
         <v>83</v>
       </c>
       <c r="E70">
-        <v>13.70907465</v>
+        <v>13.74157164</v>
       </c>
       <c r="F70">
-        <v>100.5309339</v>
+        <v>100.5295636</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -3894,10 +3909,10 @@
         <v>0</v>
       </c>
       <c r="L70" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="M70" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="N70">
         <v>0</v>
@@ -3917,10 +3932,10 @@
         <v>84</v>
       </c>
       <c r="E71">
-        <v>13.72017547</v>
+        <v>13.73967506</v>
       </c>
       <c r="F71">
-        <v>100.4569003</v>
+        <v>100.5262292</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -3938,10 +3953,10 @@
         <v>0</v>
       </c>
       <c r="L71" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="M71" s="3" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="N71">
         <v>0</v>
@@ -3961,10 +3976,10 @@
         <v>85</v>
       </c>
       <c r="E72">
-        <v>13.71423245</v>
+        <v>13.70907465</v>
       </c>
       <c r="F72">
-        <v>100.4767845</v>
+        <v>100.5309339</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -3982,10 +3997,10 @@
         <v>0</v>
       </c>
       <c r="L72" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="M72" s="3" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="N72">
         <v>0</v>
@@ -4005,10 +4020,10 @@
         <v>86</v>
       </c>
       <c r="E73">
-        <v>13.74582639</v>
+        <v>13.72017547</v>
       </c>
       <c r="F73">
-        <v>100.5325534</v>
+        <v>100.4569003</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -4026,10 +4041,10 @@
         <v>0</v>
       </c>
       <c r="L73" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="M73" s="3" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="N73">
         <v>0</v>
@@ -4043,16 +4058,16 @@
         <v>15</v>
       </c>
       <c r="C74" s="2">
-        <v>44233</v>
+        <v>44232</v>
       </c>
       <c r="D74" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E74">
-        <v>13.74181404</v>
+        <v>13.71423245</v>
       </c>
       <c r="F74">
-        <v>100.5259746</v>
+        <v>100.4767845</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -4070,10 +4085,10 @@
         <v>0</v>
       </c>
       <c r="L74" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="M74" s="3" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="N74">
         <v>0</v>
@@ -4087,16 +4102,16 @@
         <v>15</v>
       </c>
       <c r="C75" s="2">
-        <v>44233</v>
+        <v>44232</v>
       </c>
       <c r="D75" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="E75">
-        <v>13.74278916</v>
+        <v>13.74582639</v>
       </c>
       <c r="F75">
-        <v>100.5247178</v>
+        <v>100.5325534</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -4114,10 +4129,10 @@
         <v>0</v>
       </c>
       <c r="L75" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="M75" s="3" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="N75">
         <v>0</v>
@@ -4134,13 +4149,13 @@
         <v>44233</v>
       </c>
       <c r="D76" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>13.74181404</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>100.5259746</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -4158,10 +4173,10 @@
         <v>0</v>
       </c>
       <c r="L76" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="M76" s="3" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="N76">
         <v>0</v>
@@ -4178,13 +4193,13 @@
         <v>44233</v>
       </c>
       <c r="D77" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="E77">
-        <v>13.74082175</v>
+        <v>13.74278916</v>
       </c>
       <c r="F77">
-        <v>100.5184084</v>
+        <v>100.5247178</v>
       </c>
       <c r="G77">
         <v>0</v>
@@ -4202,10 +4217,10 @@
         <v>0</v>
       </c>
       <c r="L77" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M77" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N77">
         <v>0</v>
@@ -4225,10 +4240,10 @@
         <v>89</v>
       </c>
       <c r="E78">
-        <v>13.73097246</v>
+        <v>0</v>
       </c>
       <c r="F78">
-        <v>100.569653</v>
+        <v>0</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -4246,10 +4261,10 @@
         <v>0</v>
       </c>
       <c r="L78" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="M78" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="N78">
         <v>0</v>
@@ -4269,10 +4284,10 @@
         <v>90</v>
       </c>
       <c r="E79">
-        <v>13.71080935</v>
+        <v>13.74082175</v>
       </c>
       <c r="F79">
-        <v>100.5700614</v>
+        <v>100.5184084</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -4293,7 +4308,7 @@
         <v>126</v>
       </c>
       <c r="M79" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N79">
         <v>0</v>
@@ -4313,10 +4328,10 @@
         <v>91</v>
       </c>
       <c r="E80">
-        <v>13.74404607</v>
+        <v>13.73097246</v>
       </c>
       <c r="F80">
-        <v>100.5328116</v>
+        <v>100.569653</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -4334,10 +4349,10 @@
         <v>0</v>
       </c>
       <c r="L80" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="M80" s="3" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="N80">
         <v>0</v>
@@ -4354,13 +4369,13 @@
         <v>44233</v>
       </c>
       <c r="D81" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="E81">
-        <v>13.73818025</v>
+        <v>13.71080935</v>
       </c>
       <c r="F81">
-        <v>100.5289019</v>
+        <v>100.5700614</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -4378,10 +4393,10 @@
         <v>0</v>
       </c>
       <c r="L81" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="M81" s="3" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="N81">
         <v>0</v>
@@ -4398,13 +4413,13 @@
         <v>44233</v>
       </c>
       <c r="D82" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E82">
-        <v>13.7119359</v>
+        <v>13.74404607</v>
       </c>
       <c r="F82">
-        <v>100.4347272</v>
+        <v>100.5328116</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -4422,10 +4437,10 @@
         <v>0</v>
       </c>
       <c r="L82" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="M82" s="3" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="N82">
         <v>0</v>
@@ -4439,16 +4454,16 @@
         <v>15</v>
       </c>
       <c r="C83" s="2">
-        <v>44234</v>
+        <v>44233</v>
       </c>
       <c r="D83" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="E83">
-        <v>13.7407093</v>
+        <v>13.73818025</v>
       </c>
       <c r="F83">
-        <v>100.5290294</v>
+        <v>100.5289019</v>
       </c>
       <c r="G83">
         <v>0</v>
@@ -4466,10 +4481,10 @@
         <v>0</v>
       </c>
       <c r="L83" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="M83" s="3" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="N83">
         <v>0</v>
@@ -4483,16 +4498,16 @@
         <v>15</v>
       </c>
       <c r="C84" s="2">
-        <v>44234</v>
+        <v>44233</v>
       </c>
       <c r="D84" t="s">
         <v>94</v>
       </c>
       <c r="E84">
-        <v>13.7410711</v>
+        <v>13.7119359</v>
       </c>
       <c r="F84">
-        <v>100.5259049</v>
+        <v>100.4347272</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -4510,10 +4525,10 @@
         <v>0</v>
       </c>
       <c r="L84" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M84" s="3" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="N84">
         <v>0</v>
@@ -4533,10 +4548,10 @@
         <v>95</v>
       </c>
       <c r="E85">
-        <v>13.73755134</v>
+        <v>13.7407093</v>
       </c>
       <c r="F85">
-        <v>100.5605514</v>
+        <v>100.5290294</v>
       </c>
       <c r="G85">
         <v>0</v>
@@ -4557,7 +4572,7 @@
         <v>126</v>
       </c>
       <c r="M85" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N85">
         <v>0</v>
@@ -4577,10 +4592,10 @@
         <v>96</v>
       </c>
       <c r="E86">
-        <v>13.73852226</v>
+        <v>13.7410711</v>
       </c>
       <c r="F86">
-        <v>100.5606332</v>
+        <v>100.5259049</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -4601,7 +4616,7 @@
         <v>126</v>
       </c>
       <c r="M86" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="N86">
         <v>0</v>
@@ -4621,10 +4636,10 @@
         <v>97</v>
       </c>
       <c r="E87">
-        <v>13.73805302</v>
+        <v>13.73755134</v>
       </c>
       <c r="F87">
-        <v>100.5606309</v>
+        <v>100.5605514</v>
       </c>
       <c r="G87">
         <v>0</v>
@@ -4642,10 +4657,10 @@
         <v>0</v>
       </c>
       <c r="L87" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="M87" s="3" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="N87">
         <v>0</v>
@@ -4665,10 +4680,10 @@
         <v>98</v>
       </c>
       <c r="E88">
-        <v>13.74643623</v>
+        <v>13.73852226</v>
       </c>
       <c r="F88">
-        <v>100.5068449</v>
+        <v>100.5606332</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -4686,10 +4701,10 @@
         <v>0</v>
       </c>
       <c r="L88" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="M88" s="3" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="N88">
         <v>0</v>
@@ -4709,10 +4724,10 @@
         <v>99</v>
       </c>
       <c r="E89">
-        <v>13.74064474</v>
+        <v>13.73805302</v>
       </c>
       <c r="F89">
-        <v>100.5271029</v>
+        <v>100.5606309</v>
       </c>
       <c r="G89">
         <v>0</v>
@@ -4730,10 +4745,10 @@
         <v>0</v>
       </c>
       <c r="L89" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="M89" s="3" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="N89">
         <v>0</v>
@@ -4753,10 +4768,10 @@
         <v>100</v>
       </c>
       <c r="E90">
-        <v>13.67904452</v>
+        <v>13.74643623</v>
       </c>
       <c r="F90">
-        <v>100.3363908</v>
+        <v>100.5068449</v>
       </c>
       <c r="G90">
         <v>0</v>
@@ -4774,10 +4789,10 @@
         <v>0</v>
       </c>
       <c r="L90" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="M90" s="3" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="N90">
         <v>0</v>
@@ -4791,16 +4806,16 @@
         <v>15</v>
       </c>
       <c r="C91" s="2">
-        <v>44235</v>
+        <v>44234</v>
       </c>
       <c r="D91" t="s">
         <v>101</v>
       </c>
       <c r="E91">
-        <v>13.73207345</v>
+        <v>13.74064474</v>
       </c>
       <c r="F91">
-        <v>100.533142</v>
+        <v>100.5271029</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -4818,10 +4833,10 @@
         <v>0</v>
       </c>
       <c r="L91" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="M91" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="N91">
         <v>0</v>
@@ -4835,16 +4850,16 @@
         <v>15</v>
       </c>
       <c r="C92" s="2">
-        <v>44235</v>
+        <v>44234</v>
       </c>
       <c r="D92" t="s">
         <v>102</v>
       </c>
       <c r="E92">
-        <v>13.7386876</v>
+        <v>13.67904452</v>
       </c>
       <c r="F92">
-        <v>100.5346272</v>
+        <v>100.3363908</v>
       </c>
       <c r="G92">
         <v>0</v>
@@ -4865,7 +4880,7 @@
         <v>124</v>
       </c>
       <c r="M92" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N92">
         <v>0</v>
@@ -4885,10 +4900,10 @@
         <v>103</v>
       </c>
       <c r="E93">
-        <v>13.73902918</v>
+        <v>13.73207345</v>
       </c>
       <c r="F93">
-        <v>100.5344107</v>
+        <v>100.533142</v>
       </c>
       <c r="G93">
         <v>0</v>
@@ -4906,10 +4921,10 @@
         <v>0</v>
       </c>
       <c r="L93" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="M93" s="3" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="N93">
         <v>0</v>
@@ -4929,10 +4944,10 @@
         <v>104</v>
       </c>
       <c r="E94">
-        <v>13.73825721</v>
+        <v>13.7386876</v>
       </c>
       <c r="F94">
-        <v>100.5326718</v>
+        <v>100.5346272</v>
       </c>
       <c r="G94">
         <v>0</v>
@@ -4950,10 +4965,10 @@
         <v>0</v>
       </c>
       <c r="L94" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="M94" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N94">
         <v>0</v>
@@ -4967,16 +4982,16 @@
         <v>15</v>
       </c>
       <c r="C95" s="2">
-        <v>44236</v>
+        <v>44235</v>
       </c>
       <c r="D95" t="s">
         <v>105</v>
       </c>
       <c r="E95">
-        <v>13.73822735</v>
+        <v>13.73902918</v>
       </c>
       <c r="F95">
-        <v>100.5284446</v>
+        <v>100.5344107</v>
       </c>
       <c r="G95">
         <v>0</v>
@@ -4994,10 +5009,10 @@
         <v>0</v>
       </c>
       <c r="L95" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="M95" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N95">
         <v>0</v>
@@ -5011,16 +5026,16 @@
         <v>15</v>
       </c>
       <c r="C96" s="2">
-        <v>44236</v>
+        <v>44235</v>
       </c>
       <c r="D96" t="s">
         <v>106</v>
       </c>
       <c r="E96">
-        <v>13.71216883</v>
+        <v>13.73825721</v>
       </c>
       <c r="F96">
-        <v>100.4886336</v>
+        <v>100.5326718</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -5038,10 +5053,10 @@
         <v>0</v>
       </c>
       <c r="L96" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="M96" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N96">
         <v>0</v>
@@ -5061,10 +5076,10 @@
         <v>107</v>
       </c>
       <c r="E97">
-        <v>13.72441648</v>
+        <v>13.73822735</v>
       </c>
       <c r="F97">
-        <v>100.4930201</v>
+        <v>100.5284446</v>
       </c>
       <c r="G97">
         <v>0</v>
@@ -5082,10 +5097,10 @@
         <v>0</v>
       </c>
       <c r="L97" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="M97" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N97">
         <v>0</v>
@@ -5099,16 +5114,16 @@
         <v>15</v>
       </c>
       <c r="C98" s="2">
-        <v>44237</v>
+        <v>44236</v>
       </c>
       <c r="D98" t="s">
         <v>108</v>
       </c>
       <c r="E98">
-        <v>13.74243313</v>
+        <v>13.71216883</v>
       </c>
       <c r="F98">
-        <v>100.533686</v>
+        <v>100.4886336</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -5126,10 +5141,10 @@
         <v>0</v>
       </c>
       <c r="L98" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="M98" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N98">
         <v>0</v>
@@ -5143,16 +5158,16 @@
         <v>15</v>
       </c>
       <c r="C99" s="2">
-        <v>44237</v>
+        <v>44236</v>
       </c>
       <c r="D99" t="s">
         <v>109</v>
       </c>
       <c r="E99">
-        <v>13.74007973</v>
+        <v>13.72441648</v>
       </c>
       <c r="F99">
-        <v>100.5246268</v>
+        <v>100.4930201</v>
       </c>
       <c r="G99">
         <v>0</v>
@@ -5170,10 +5185,10 @@
         <v>0</v>
       </c>
       <c r="L99" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="M99" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="N99">
         <v>0</v>
@@ -5193,33 +5208,165 @@
         <v>110</v>
       </c>
       <c r="E100">
+        <v>13.74243313</v>
+      </c>
+      <c r="F100">
+        <v>100.533686</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+      <c r="K100">
+        <v>0</v>
+      </c>
+      <c r="L100" t="s">
+        <v>127</v>
+      </c>
+      <c r="M100" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="N100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" s="2">
+        <v>44237</v>
+      </c>
+      <c r="D101" t="s">
+        <v>111</v>
+      </c>
+      <c r="E101">
+        <v>13.74007973</v>
+      </c>
+      <c r="F101">
+        <v>100.5246268</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101">
+        <v>0</v>
+      </c>
+      <c r="J101">
+        <v>0</v>
+      </c>
+      <c r="K101">
+        <v>0</v>
+      </c>
+      <c r="L101" t="s">
+        <v>127</v>
+      </c>
+      <c r="M101" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="N101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>15</v>
+      </c>
+      <c r="C102" s="2">
+        <v>44237</v>
+      </c>
+      <c r="D102" t="s">
+        <v>112</v>
+      </c>
+      <c r="E102">
         <v>13.96212333</v>
       </c>
-      <c r="F100">
+      <c r="F102">
         <v>100.6186288</v>
       </c>
-      <c r="G100">
-        <v>0</v>
-      </c>
-      <c r="H100">
-        <v>0</v>
-      </c>
-      <c r="I100">
-        <v>0</v>
-      </c>
-      <c r="J100">
-        <v>0</v>
-      </c>
-      <c r="K100">
-        <v>0</v>
-      </c>
-      <c r="L100" t="s">
-        <v>121</v>
-      </c>
-      <c r="M100" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="N100">
+      <c r="G102">
+        <v>0</v>
+      </c>
+      <c r="H102">
+        <v>0</v>
+      </c>
+      <c r="I102">
+        <v>0</v>
+      </c>
+      <c r="J102">
+        <v>0</v>
+      </c>
+      <c r="K102">
+        <v>0</v>
+      </c>
+      <c r="L102" t="s">
+        <v>124</v>
+      </c>
+      <c r="M102" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="N102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>15</v>
+      </c>
+      <c r="C103" s="2">
+        <v>44238</v>
+      </c>
+      <c r="D103" t="s">
+        <v>113</v>
+      </c>
+      <c r="E103">
+        <v>13.73378448</v>
+      </c>
+      <c r="F103">
+        <v>100.5024518</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <v>0</v>
+      </c>
+      <c r="I103">
+        <v>0</v>
+      </c>
+      <c r="J103">
+        <v>0</v>
+      </c>
+      <c r="K103">
+        <v>0</v>
+      </c>
+      <c r="L103" t="s">
+        <v>129</v>
+      </c>
+      <c r="M103" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="N103">
         <v>0</v>
       </c>
     </row>
@@ -5324,6 +5471,9 @@
     <hyperlink ref="M98" r:id="rId97"/>
     <hyperlink ref="M99" r:id="rId98"/>
     <hyperlink ref="M100" r:id="rId99"/>
+    <hyperlink ref="M101" r:id="rId100"/>
+    <hyperlink ref="M102" r:id="rId101"/>
+    <hyperlink ref="M103" r:id="rId102"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>